<commit_message>
aggiornamento 5 - 29.09.2029
Aggiornamento 5 -29-09-2029
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DATASOFTNA/DATASOFT/LABGUI/3.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111DATASOFTNA/DATASOFT/LABGUI/3.0/report-checklist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="195">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -464,7 +464,7 @@
     <t xml:space="preserve">Viene visualizzata la risposta del gateway+Viene avvisato l’inviante che c’e’ un errore strutturale e di avvisare il fornitore del software l’errore non inficia la creazione del referto in quanto la trasmissione e’ posteriore+ viene registrata in un file di log+la richiesta viene inserita tra quelle da ritrasmettere</t>
   </si>
   <si>
-    <t xml:space="preserve">Viene rilevata la segnalazione da parte dell’inviante e corretto l’errore del software da parte di Datasoft</t>
+    <t xml:space="preserve">Apertura di ticket e analisi del log</t>
   </si>
   <si>
     <t xml:space="preserve">KO</t>
@@ -555,7 +555,7 @@
     <t xml:space="preserve">Viene segnalato all’INVIANTE che si e’ verificato un TIMEOUT e puo’ provare a ritentare e a controllare lo stato della connessione internet +  l’evento viene registrato nel log+la richiesta viene inserita tra quelle da ritrasmettere+se l’operazione non e’ interattiva, l’inviante consulta il log</t>
   </si>
   <si>
-    <t xml:space="preserve">Viene chiesto all’inviante di controllare la sua connessione internet e se gli e’ possibile, verificare se l’endpoint e’ attivo</t>
+    <t xml:space="preserve">Viene suggerito all’inviante di controllare la sua connessione internet e se gli e’ possibile, verificare se l’endpoint e’ attivo</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LAB_CT6_KO</t>
@@ -654,10 +654,7 @@
     <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.092424a8b83ac1734d0e118a4c3a43c793f3f6c63b6ba838d480115903a3b457.0e8346143a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t xml:space="preserve">Viene visualizzata la risposta del gateway alla persona che sta effettuando la trasmissione + viene registrata in un file di log</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All’INVIANTE viene visualizzata la risposta del Gateway.+Richiesta di contattare il fornitore del software.</t>
+    <t xml:space="preserve">Viene visualizzata la risposta del gateway alla persona che sta effettuando la trasmissione + viene registrata in un file di log+richiesta di contattare il fornitore</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LAB_CT15_KO</t>
@@ -684,9 +681,6 @@
   </si>
   <si>
     <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.687d9ade5891f6681a5a8231ce0d4ac16be6cb2e3ab9e2b490ad662dff2b34fa.a9ea1d1558^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L’errore viene gestito richiedendo all’INVIANTE di contattare il fornitore del software, dato che si tratta di una situazione anomala che non puo’ dipendere da qualche sua azione+la richiesta viene inserita tra quelle da ritrasmettere</t>
   </si>
   <si>
     <t xml:space="preserve">ID TEST CASE OK</t>
@@ -2075,9 +2069,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>99720</xdr:colOff>
+      <xdr:colOff>99360</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>939600</xdr:rowOff>
+      <xdr:rowOff>939240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2087,7 +2081,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5370840" cy="2889360"/>
+          <a:ext cx="5370480" cy="2889000"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4330,11 +4324,11 @@
   <dimension ref="A1:T959"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="J22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
-      <selection pane="bottomRight" activeCell="O27" activeCellId="0" sqref="O27"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="P18" activeCellId="0" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5318,7 +5312,7 @@
         <v>56</v>
       </c>
       <c r="P26" s="32" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="Q26" s="32"/>
       <c r="R26" s="33"/>
@@ -5338,10 +5332,10 @@
         <v>49</v>
       </c>
       <c r="D27" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="E27" s="29" t="s">
         <v>128</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>129</v>
       </c>
       <c r="F27" s="30"/>
       <c r="G27" s="30"/>
@@ -5351,7 +5345,7 @@
         <v>92</v>
       </c>
       <c r="K27" s="32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L27" s="32"/>
       <c r="M27" s="32"/>
@@ -5376,22 +5370,22 @@
         <v>49</v>
       </c>
       <c r="D28" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="E28" s="29" t="s">
         <v>131</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>132</v>
       </c>
       <c r="F28" s="30" t="n">
         <v>45082</v>
       </c>
       <c r="G28" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="H28" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="H28" s="31" t="s">
+      <c r="I28" s="31" t="s">
         <v>134</v>
-      </c>
-      <c r="I28" s="31" t="s">
-        <v>135</v>
       </c>
       <c r="J28" s="32" t="s">
         <v>56</v>
@@ -5410,7 +5404,7 @@
         <v>56</v>
       </c>
       <c r="P28" s="32" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="Q28" s="32"/>
       <c r="R28" s="33"/>
@@ -17041,10 +17035,10 @@
         <v>29</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17052,125 +17046,125 @@
         <v>49</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="38" t="s">
         <v>139</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>140</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="38" t="s">
         <v>142</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" s="39" t="s">
         <v>145</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="38" t="s">
         <v>148</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>149</v>
-      </c>
-      <c r="D5" s="38" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="39" t="s">
         <v>151</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="D6" s="39" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="39" t="s">
         <v>154</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>155</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="39" t="s">
         <v>157</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C8" s="38" t="s">
-        <v>158</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="39" t="s">
         <v>160</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" s="38" t="s">
         <v>163</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>164</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17178,111 +17172,111 @@
         <v>49</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C11" s="38" t="n">
         <v>192</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C12" s="38" t="n">
         <v>208</v>
       </c>
       <c r="D12" s="38" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C13" s="38" t="n">
         <v>224</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C14" s="38" t="n">
         <v>240</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C15" s="38" t="n">
         <v>256</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C16" s="38" t="n">
         <v>272</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C17" s="38" t="n">
         <v>288</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C18" s="38" t="n">
         <v>304</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17290,111 +17284,111 @@
         <v>49</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C19" s="38" t="n">
         <v>193</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C20" s="38" t="n">
         <v>209</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C21" s="38" t="n">
         <v>225</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C22" s="38" t="n">
         <v>241</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C23" s="38" t="n">
         <v>257</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C24" s="38" t="n">
         <v>273</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C25" s="38" t="n">
         <v>289</v>
       </c>
       <c r="D25" s="39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C26" s="38" t="n">
         <v>305</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17402,111 +17396,111 @@
         <v>49</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C27" s="38" t="n">
         <v>194</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C28" s="38" t="n">
         <v>210</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C29" s="38" t="n">
         <v>226</v>
       </c>
       <c r="D29" s="40" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C30" s="38" t="n">
         <v>242</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C31" s="38" t="n">
         <v>258</v>
       </c>
       <c r="D31" s="39" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C32" s="38" t="n">
         <v>274</v>
       </c>
       <c r="D32" s="39" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C33" s="38" t="n">
         <v>290</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C34" s="38" t="n">
         <v>306</v>
       </c>
       <c r="D34" s="39" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17514,7 +17508,7 @@
         <v>49</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C35" s="38" t="n">
         <v>195</v>
@@ -17525,10 +17519,10 @@
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C36" s="38" t="n">
         <v>211</v>
@@ -17539,10 +17533,10 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C37" s="38" t="n">
         <v>227</v>
@@ -17553,10 +17547,10 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C38" s="38" t="n">
         <v>243</v>
@@ -17567,10 +17561,10 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C39" s="38" t="n">
         <v>259</v>
@@ -17581,10 +17575,10 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C40" s="38" t="n">
         <v>275</v>
@@ -17595,10 +17589,10 @@
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C41" s="38" t="n">
         <v>291</v>
@@ -17609,10 +17603,10 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C42" s="38" t="n">
         <v>307</v>
@@ -17626,7 +17620,7 @@
         <v>49</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C43" s="38" t="n">
         <v>196</v>
@@ -17637,10 +17631,10 @@
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C44" s="38" t="n">
         <v>212</v>
@@ -17651,10 +17645,10 @@
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C45" s="38" t="n">
         <v>228</v>
@@ -17665,10 +17659,10 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C46" s="38" t="n">
         <v>244</v>
@@ -17679,10 +17673,10 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C47" s="38" t="n">
         <v>260</v>
@@ -17693,10 +17687,10 @@
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C48" s="38" t="n">
         <v>276</v>
@@ -17707,10 +17701,10 @@
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C49" s="38" t="n">
         <v>292</v>
@@ -17721,10 +17715,10 @@
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C50" s="38" t="n">
         <v>308</v>
@@ -18723,7 +18717,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="41" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B2" s="41" t="s">
         <v>56</v>
@@ -18731,7 +18725,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="41" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B3" s="41" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
Aggiornato report-checklist.xlsx - 9 29.09.2029
Aggiornato report-checklist.xlsx - 9  29.09.2029
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DATASOFTNA/DATASOFT/LABGUI/3.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111DATASOFTNA/DATASOFT/LABGUI/3.0/report-checklist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="194">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -461,7 +461,7 @@
     <t xml:space="preserve">UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Viene visualizzata la risposta del gateway+Viene avvisato l’inviante che c’e’ un errore strutturale e di avvisare il fornitore del software l’errore non inficia la creazione del referto in quanto la trasmissione e’ posteriore+ viene registrata in un file di log+la richiesta viene inserita tra quelle da ritrasmettere</t>
+    <t xml:space="preserve">Errore dell’applicativo contattare  il fornitore</t>
   </si>
   <si>
     <t xml:space="preserve">Apertura di ticket e analisi del log</t>
@@ -542,9 +542,6 @@
     <t xml:space="preserve">a0fc8f87aabeb7ba</t>
   </si>
   <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
     <t xml:space="preserve">VALIDAZIONE_LAB_TIMEOUT</t>
   </si>
   <si>
@@ -552,7 +549,7 @@
 "ERRORE BLOCCANTE (SI/NO)", "ERRORE VISIBILE A UTENTE (SI/NO)", "MESSAGGIO DI ERRORE", "GESTITO IN BACKOFFICE (SI/NO)", "GESTIONE ERRORE".</t>
   </si>
   <si>
-    <t xml:space="preserve">Viene segnalato all’INVIANTE che si e’ verificato un TIMEOUT e puo’ provare a ritentare e a controllare lo stato della connessione internet +  l’evento viene registrato nel log+la richiesta viene inserita tra quelle da ritrasmettere+se l’operazione non e’ interattiva, l’inviante consulta il log</t>
+    <t xml:space="preserve">Tineout riprovare piu’ tardi e controllare la connessione internet</t>
   </si>
   <si>
     <t xml:space="preserve">Viene suggerito all’inviante di controllare la sua connessione internet e se gli e’ possibile, verificare se l’endpoint e’ attivo</t>
@@ -563,6 +560,9 @@
   <si>
     <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori sintattici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
   </si>
   <si>
     <t xml:space="preserve">Non è possibile produrre un referto per i pazienti senza confidentiality code</t>
@@ -652,9 +652,6 @@
   </si>
   <si>
     <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.092424a8b83ac1734d0e118a4c3a43c793f3f6c63b6ba838d480115903a3b457.0e8346143a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viene visualizzata la risposta del gateway alla persona che sta effettuando la trasmissione + viene registrata in un file di log+richiesta di contattare il fornitore</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LAB_CT15_KO</t>
@@ -872,7 +869,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="D/M/YYYY"/>
   </numFmts>
-  <fonts count="40">
+  <fonts count="41">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1168,6 +1165,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="23">
@@ -1759,7 +1762,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1909,6 +1912,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2069,9 +2076,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>99360</xdr:colOff>
+      <xdr:colOff>99000</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>939240</xdr:rowOff>
+      <xdr:rowOff>938880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2081,7 +2088,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="5370480" cy="2889000"/>
+          <a:ext cx="5370120" cy="2888640"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4324,11 +4331,11 @@
   <dimension ref="A1:T959"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="I10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="I31" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="P18" activeCellId="0" sqref="P18"/>
+      <selection pane="bottomLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="N28" activeCellId="0" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4905,7 +4912,7 @@
         <v>85</v>
       </c>
       <c r="O16" s="32" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="P16" s="32" t="s">
         <v>86</v>
@@ -4917,7 +4924,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="27" t="n">
         <v>44</v>
       </c>
@@ -4928,10 +4935,10 @@
         <v>49</v>
       </c>
       <c r="D17" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="29" t="s">
         <v>93</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>94</v>
       </c>
       <c r="F17" s="30"/>
       <c r="G17" s="31"/>
@@ -4948,13 +4955,13 @@
         <v>56</v>
       </c>
       <c r="N17" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="O17" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="P17" s="32" t="s">
         <v>95</v>
-      </c>
-      <c r="O17" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="P17" s="32" t="s">
-        <v>96</v>
       </c>
       <c r="Q17" s="32"/>
       <c r="R17" s="33"/>
@@ -4974,17 +4981,17 @@
         <v>49</v>
       </c>
       <c r="D18" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="29" t="s">
         <v>97</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>98</v>
       </c>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
       <c r="H18" s="31"/>
       <c r="I18" s="31"/>
       <c r="J18" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K18" s="32" t="s">
         <v>99</v>
@@ -5022,7 +5029,7 @@
       <c r="H19" s="31"/>
       <c r="I19" s="31"/>
       <c r="J19" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K19" s="32" t="s">
         <v>102</v>
@@ -5060,7 +5067,7 @@
       <c r="H20" s="31"/>
       <c r="I20" s="31"/>
       <c r="J20" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K20" s="32" t="s">
         <v>105</v>
@@ -5098,7 +5105,7 @@
       <c r="H21" s="31"/>
       <c r="I21" s="31"/>
       <c r="J21" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K21" s="37" t="s">
         <v>108</v>
@@ -5136,7 +5143,7 @@
       <c r="H22" s="31"/>
       <c r="I22" s="31"/>
       <c r="J22" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K22" s="32" t="s">
         <v>111</v>
@@ -5174,7 +5181,7 @@
       <c r="H23" s="31"/>
       <c r="I23" s="31"/>
       <c r="J23" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K23" s="32" t="s">
         <v>114</v>
@@ -5212,7 +5219,7 @@
       <c r="H24" s="31"/>
       <c r="I24" s="31"/>
       <c r="J24" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K24" s="32" t="s">
         <v>117</v>
@@ -5250,7 +5257,7 @@
       <c r="H25" s="31"/>
       <c r="I25" s="31"/>
       <c r="J25" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K25" s="32" t="s">
         <v>120</v>
@@ -5306,7 +5313,7 @@
         <v>56</v>
       </c>
       <c r="N26" s="32" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="O26" s="32" t="s">
         <v>56</v>
@@ -5332,20 +5339,20 @@
         <v>49</v>
       </c>
       <c r="D27" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" s="29" t="s">
         <v>127</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>128</v>
       </c>
       <c r="F27" s="30"/>
       <c r="G27" s="30"/>
       <c r="H27" s="31"/>
       <c r="I27" s="31"/>
       <c r="J27" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="K27" s="32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L27" s="32"/>
       <c r="M27" s="32"/>
@@ -5370,22 +5377,22 @@
         <v>49</v>
       </c>
       <c r="D28" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="E28" s="29" t="s">
         <v>130</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>131</v>
       </c>
       <c r="F28" s="30" t="n">
         <v>45082</v>
       </c>
       <c r="G28" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="H28" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="H28" s="31" t="s">
+      <c r="I28" s="31" t="s">
         <v>133</v>
-      </c>
-      <c r="I28" s="31" t="s">
-        <v>134</v>
       </c>
       <c r="J28" s="32" t="s">
         <v>56</v>
@@ -5397,8 +5404,8 @@
       <c r="M28" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="N28" s="32" t="s">
-        <v>126</v>
+      <c r="N28" s="38" t="s">
+        <v>85</v>
       </c>
       <c r="O28" s="32" t="s">
         <v>56</v>
@@ -17035,10 +17042,10 @@
         <v>29</v>
       </c>
       <c r="C1" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>135</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17046,125 +17053,125 @@
         <v>49</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="D2" s="39" t="s">
         <v>138</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3" s="38" t="s">
+      <c r="D3" s="39" t="s">
         <v>141</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" s="38" t="s">
+      <c r="D4" s="40" t="s">
         <v>144</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C5" s="38" t="s">
+      <c r="D5" s="39" t="s">
         <v>147</v>
-      </c>
-      <c r="D5" s="38" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" s="38" t="s">
+      <c r="D6" s="40" t="s">
         <v>150</v>
-      </c>
-      <c r="D6" s="39" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C7" s="38" t="s">
+      <c r="D7" s="40" t="s">
         <v>153</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C8" s="38" t="s">
+      <c r="D8" s="40" t="s">
         <v>156</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C9" s="38" t="s">
+      <c r="D9" s="40" t="s">
         <v>159</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="40" t="s">
         <v>161</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C10" s="39" t="s">
+      <c r="D10" s="39" t="s">
         <v>162</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17172,111 +17179,111 @@
         <v>49</v>
       </c>
       <c r="B11" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="39" t="n">
+        <v>192</v>
+      </c>
+      <c r="D11" s="39" t="s">
         <v>164</v>
-      </c>
-      <c r="C11" s="38" t="n">
-        <v>192</v>
-      </c>
-      <c r="D11" s="38" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C12" s="38" t="n">
+        <v>163</v>
+      </c>
+      <c r="C12" s="39" t="n">
         <v>208</v>
       </c>
-      <c r="D12" s="38" t="s">
-        <v>166</v>
+      <c r="D12" s="39" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C13" s="38" t="n">
+        <v>163</v>
+      </c>
+      <c r="C13" s="39" t="n">
         <v>224</v>
       </c>
-      <c r="D13" s="39" t="s">
-        <v>167</v>
+      <c r="D13" s="40" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C14" s="38" t="n">
+        <v>163</v>
+      </c>
+      <c r="C14" s="39" t="n">
         <v>240</v>
       </c>
-      <c r="D14" s="38" t="s">
-        <v>168</v>
+      <c r="D14" s="39" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C15" s="38" t="n">
+        <v>163</v>
+      </c>
+      <c r="C15" s="39" t="n">
         <v>256</v>
       </c>
-      <c r="D15" s="39" t="s">
-        <v>169</v>
+      <c r="D15" s="40" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C16" s="38" t="n">
+        <v>163</v>
+      </c>
+      <c r="C16" s="39" t="n">
         <v>272</v>
       </c>
-      <c r="D16" s="39" t="s">
-        <v>170</v>
+      <c r="D16" s="40" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C17" s="38" t="n">
+        <v>163</v>
+      </c>
+      <c r="C17" s="39" t="n">
         <v>288</v>
       </c>
-      <c r="D17" s="39" t="s">
-        <v>171</v>
+      <c r="D17" s="40" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C18" s="38" t="n">
+        <v>163</v>
+      </c>
+      <c r="C18" s="39" t="n">
         <v>304</v>
       </c>
-      <c r="D18" s="39" t="s">
-        <v>172</v>
+      <c r="D18" s="40" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17284,111 +17291,111 @@
         <v>49</v>
       </c>
       <c r="B19" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="39" t="n">
+        <v>193</v>
+      </c>
+      <c r="D19" s="39" t="s">
         <v>173</v>
-      </c>
-      <c r="C19" s="38" t="n">
-        <v>193</v>
-      </c>
-      <c r="D19" s="38" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C20" s="38" t="n">
+        <v>172</v>
+      </c>
+      <c r="C20" s="39" t="n">
         <v>209</v>
       </c>
-      <c r="D20" s="38" t="s">
-        <v>175</v>
+      <c r="D20" s="39" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C21" s="38" t="n">
+        <v>172</v>
+      </c>
+      <c r="C21" s="39" t="n">
         <v>225</v>
       </c>
-      <c r="D21" s="39" t="s">
-        <v>176</v>
+      <c r="D21" s="40" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C22" s="38" t="n">
+        <v>172</v>
+      </c>
+      <c r="C22" s="39" t="n">
         <v>241</v>
       </c>
-      <c r="D22" s="38" t="s">
-        <v>177</v>
+      <c r="D22" s="39" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C23" s="38" t="n">
+        <v>172</v>
+      </c>
+      <c r="C23" s="39" t="n">
         <v>257</v>
       </c>
-      <c r="D23" s="39" t="s">
-        <v>178</v>
+      <c r="D23" s="40" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C24" s="38" t="n">
+        <v>172</v>
+      </c>
+      <c r="C24" s="39" t="n">
         <v>273</v>
       </c>
-      <c r="D24" s="39" t="s">
-        <v>179</v>
+      <c r="D24" s="40" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C25" s="38" t="n">
+        <v>172</v>
+      </c>
+      <c r="C25" s="39" t="n">
         <v>289</v>
       </c>
-      <c r="D25" s="39" t="s">
-        <v>180</v>
+      <c r="D25" s="40" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C26" s="38" t="n">
+        <v>172</v>
+      </c>
+      <c r="C26" s="39" t="n">
         <v>305</v>
       </c>
-      <c r="D26" s="39" t="s">
-        <v>181</v>
+      <c r="D26" s="40" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17396,111 +17403,111 @@
         <v>49</v>
       </c>
       <c r="B27" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="C27" s="39" t="n">
+        <v>194</v>
+      </c>
+      <c r="D27" s="39" t="s">
         <v>182</v>
-      </c>
-      <c r="C27" s="38" t="n">
-        <v>194</v>
-      </c>
-      <c r="D27" s="38" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C28" s="38" t="n">
+        <v>181</v>
+      </c>
+      <c r="C28" s="39" t="n">
         <v>210</v>
       </c>
-      <c r="D28" s="38" t="s">
-        <v>184</v>
+      <c r="D28" s="39" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C29" s="38" t="n">
+        <v>181</v>
+      </c>
+      <c r="C29" s="39" t="n">
         <v>226</v>
       </c>
-      <c r="D29" s="40" t="s">
-        <v>185</v>
+      <c r="D29" s="41" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C30" s="38" t="n">
+        <v>181</v>
+      </c>
+      <c r="C30" s="39" t="n">
         <v>242</v>
       </c>
-      <c r="D30" s="38" t="s">
-        <v>186</v>
+      <c r="D30" s="39" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C31" s="38" t="n">
+        <v>181</v>
+      </c>
+      <c r="C31" s="39" t="n">
         <v>258</v>
       </c>
-      <c r="D31" s="39" t="s">
-        <v>187</v>
+      <c r="D31" s="40" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C32" s="38" t="n">
+        <v>181</v>
+      </c>
+      <c r="C32" s="39" t="n">
         <v>274</v>
       </c>
-      <c r="D32" s="39" t="s">
-        <v>188</v>
+      <c r="D32" s="40" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C33" s="38" t="n">
+        <v>181</v>
+      </c>
+      <c r="C33" s="39" t="n">
         <v>290</v>
       </c>
-      <c r="D33" s="39" t="s">
-        <v>189</v>
+      <c r="D33" s="40" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C34" s="38" t="n">
+        <v>181</v>
+      </c>
+      <c r="C34" s="39" t="n">
         <v>306</v>
       </c>
-      <c r="D34" s="39" t="s">
-        <v>190</v>
+      <c r="D34" s="40" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17508,110 +17515,110 @@
         <v>49</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C35" s="38" t="n">
+        <v>190</v>
+      </c>
+      <c r="C35" s="39" t="n">
         <v>195</v>
       </c>
-      <c r="D35" s="38" t="n">
+      <c r="D35" s="39" t="n">
         <v>204</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C36" s="38" t="n">
+        <v>190</v>
+      </c>
+      <c r="C36" s="39" t="n">
         <v>211</v>
       </c>
-      <c r="D36" s="38" t="n">
+      <c r="D36" s="39" t="n">
         <v>220</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C37" s="38" t="n">
+        <v>190</v>
+      </c>
+      <c r="C37" s="39" t="n">
         <v>227</v>
       </c>
-      <c r="D37" s="39" t="n">
+      <c r="D37" s="40" t="n">
         <v>236</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C38" s="38" t="n">
+        <v>190</v>
+      </c>
+      <c r="C38" s="39" t="n">
         <v>243</v>
       </c>
-      <c r="D38" s="38" t="n">
+      <c r="D38" s="39" t="n">
         <v>252</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C39" s="38" t="n">
+        <v>190</v>
+      </c>
+      <c r="C39" s="39" t="n">
         <v>259</v>
       </c>
-      <c r="D39" s="39" t="n">
+      <c r="D39" s="40" t="n">
         <v>268</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C40" s="38" t="n">
+        <v>190</v>
+      </c>
+      <c r="C40" s="39" t="n">
         <v>275</v>
       </c>
-      <c r="D40" s="39" t="n">
+      <c r="D40" s="40" t="n">
         <v>284</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C41" s="38" t="n">
+        <v>190</v>
+      </c>
+      <c r="C41" s="39" t="n">
         <v>291</v>
       </c>
-      <c r="D41" s="39" t="n">
+      <c r="D41" s="40" t="n">
         <v>300</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="C42" s="38" t="n">
+        <v>190</v>
+      </c>
+      <c r="C42" s="39" t="n">
         <v>307</v>
       </c>
-      <c r="D42" s="39" t="n">
+      <c r="D42" s="40" t="n">
         <v>316</v>
       </c>
     </row>
@@ -17620,110 +17627,110 @@
         <v>49</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C43" s="38" t="n">
+        <v>191</v>
+      </c>
+      <c r="C43" s="39" t="n">
         <v>196</v>
       </c>
-      <c r="D43" s="38" t="n">
+      <c r="D43" s="39" t="n">
         <v>207</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C44" s="38" t="n">
+        <v>191</v>
+      </c>
+      <c r="C44" s="39" t="n">
         <v>212</v>
       </c>
-      <c r="D44" s="38" t="n">
+      <c r="D44" s="39" t="n">
         <v>223</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C45" s="38" t="n">
+        <v>191</v>
+      </c>
+      <c r="C45" s="39" t="n">
         <v>228</v>
       </c>
-      <c r="D45" s="39" t="n">
+      <c r="D45" s="40" t="n">
         <v>239</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C46" s="38" t="n">
+        <v>191</v>
+      </c>
+      <c r="C46" s="39" t="n">
         <v>244</v>
       </c>
-      <c r="D46" s="38" t="n">
+      <c r="D46" s="39" t="n">
         <v>255</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C47" s="38" t="n">
+        <v>191</v>
+      </c>
+      <c r="C47" s="39" t="n">
         <v>260</v>
       </c>
-      <c r="D47" s="39" t="n">
+      <c r="D47" s="40" t="n">
         <v>271</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C48" s="38" t="n">
+        <v>191</v>
+      </c>
+      <c r="C48" s="39" t="n">
         <v>276</v>
       </c>
-      <c r="D48" s="39" t="n">
+      <c r="D48" s="40" t="n">
         <v>287</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C49" s="38" t="n">
+        <v>191</v>
+      </c>
+      <c r="C49" s="39" t="n">
         <v>292</v>
       </c>
-      <c r="D49" s="39" t="n">
+      <c r="D49" s="40" t="n">
         <v>303</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="C50" s="38" t="n">
+        <v>191</v>
+      </c>
+      <c r="C50" s="39" t="n">
         <v>308</v>
       </c>
-      <c r="D50" s="39" t="n">
+      <c r="D50" s="40" t="n">
         <v>319</v>
       </c>
     </row>
@@ -18708,27 +18715,27 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="42" t="s">
         <v>193</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="41" t="s">
-        <v>194</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>92</v>
+      <c r="B3" s="42" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>